<commit_message>
[EI-1214] Add two new field types (Label, GPS) to New Project from Data Dictionary.
</commit_message>
<xml_diff>
--- a/Epi.Windows.MakeView/Excel/Survey.xlsx
+++ b/Epi.Windows.MakeView/Excel/Survey.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFSCode\Epi Info 7\Epi.Windows.MakeView\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mii0\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
   <si>
     <t>Question</t>
   </si>
@@ -129,18 +129,6 @@
     <t>Pregnant</t>
   </si>
   <si>
-    <t>Please enter Age ….</t>
-  </si>
-  <si>
-    <t>Please enter Name….</t>
-  </si>
-  <si>
-    <t>Please enter Sex….</t>
-  </si>
-  <si>
-    <t>Please enter Pregnant...</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -156,15 +144,9 @@
     <t>Symptoms Date</t>
   </si>
   <si>
-    <t>Please enter symptoms date…</t>
-  </si>
-  <si>
     <t>Symptoms Time</t>
   </si>
   <si>
-    <t>Please enter symptoms time…</t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
@@ -207,9 +189,6 @@
     <t>Select eaten foods:</t>
   </si>
   <si>
-    <t>Please select eaten foods…</t>
-  </si>
-  <si>
     <t>Was patient hospitalized?</t>
   </si>
   <si>
@@ -220,6 +199,33 @@
   </si>
   <si>
     <t>onset_time</t>
+  </si>
+  <si>
+    <t>GPS</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Welcome to the outbreak questionnaire</t>
+  </si>
+  <si>
+    <t>Use this space to provide additional instructions to the interviewer</t>
+  </si>
+  <si>
+    <t>label1</t>
+  </si>
+  <si>
+    <t>Where is the interview occurring?</t>
+  </si>
+  <si>
+    <t>Interview GPS</t>
+  </si>
+  <si>
+    <t>interview_gps</t>
+  </si>
+  <si>
+    <t>Welcome</t>
   </si>
 </sst>
 </file>
@@ -263,9 +269,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,17 +553,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.140625" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" customWidth="1"/>
+    <col min="3" max="3" width="61.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
@@ -570,7 +577,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>28</v>
@@ -591,99 +598,75 @@
         <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
       </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -691,39 +674,45 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
         <v>26</v>
-      </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -731,50 +720,81 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="F8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" t="s">
-        <v>47</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
       </c>
-      <c r="G9" t="s">
-        <v>55</v>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -807,17 +827,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -837,27 +857,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -902,10 +922,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,7 +967,17 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>